<commit_message>
from excel sheet scenario outline
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium_Workspace\CucmberNopCommerce\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EC1835-5A26-4465-B8AF-47C0C6F89FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EFC5B9-D8DE-4DBF-958E-D83567D01986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25095" yWindow="3705" windowWidth="21600" windowHeight="11235" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,24 +94,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,30 +139,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,7 +467,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,57 +489,57 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>